<commit_message>
#527 tabla de servicios
Se hace commit de la informacion que necesita la tabla de servicios.
</commit_message>
<xml_diff>
--- a/1.DOCUMENTACION/CODIGO/TablaServicios.xlsx
+++ b/1.DOCUMENTACION/CODIGO/TablaServicios.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17927"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cristian\Desktop\Pacto-de-Honor\1.DOCUMENTACION\CODIGO\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="20115" windowHeight="7740"/>
+    <workbookView xWindow="2016" yWindow="96" windowWidth="20112" windowHeight="7740"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -21,7 +26,7 @@
     <author>Juan Nicolas Rubiano Obando</author>
   </authors>
   <commentList>
-    <comment ref="F3" authorId="0">
+    <comment ref="F3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -51,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Fecha solicitud</t>
   </si>
@@ -84,12 +89,33 @@
   </si>
   <si>
     <t>No. Servicio</t>
+  </si>
+  <si>
+    <t>Juan Camilo Lancheros</t>
+  </si>
+  <si>
+    <t>Cristian Garzon</t>
+  </si>
+  <si>
+    <t>Nuevo</t>
+  </si>
+  <si>
+    <t>var desbloqueoAlfaNumerico=  {"id_jugador":{
+                 "id_personaje": "codigoAlfa",
+  "estado":"0" }
+};</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El servicio nos brindara el desbloueo del personaje personaje, cumpliendo si el codigo aun es valido por la fecha y si no esta desbloqueado el personaje. </t>
+  </si>
+  <si>
+    <t>id_jugador= sera el id de cada usuario en el jugo. Id_personaje= sera la informacion de el personaje que se desbloqueara. codigoAlfa = al codigo alfanumericos que se ha regalado.  Estado= Nos dira si esta desbloqueado o no este personaje.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -355,7 +381,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -378,35 +404,41 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -417,6 +449,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -465,7 +500,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -498,9 +533,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -533,6 +585,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -711,82 +780,98 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="1"/>
-    <col min="2" max="2" width="14.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.42578125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.44140625" style="1"/>
+    <col min="2" max="2" width="14.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="28.88671875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="23.33203125" style="1" customWidth="1"/>
     <col min="8" max="8" width="16" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="28.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="24" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="11.42578125" style="1"/>
+    <col min="9" max="9" width="34.33203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="33.88671875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="45.109375" style="1" customWidth="1"/>
+    <col min="12" max="12" width="12.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="11.44140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G2" s="13" t="s">
+    <row r="1" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:11" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G2" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="14"/>
-    </row>
-    <row r="3" spans="2:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="12" t="s">
+      <c r="H2" s="17"/>
+    </row>
+    <row r="3" spans="2:11" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="E3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="F3" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="12" t="s">
+      <c r="G3" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="12" t="s">
+      <c r="H3" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="I3" s="12" t="s">
+      <c r="I3" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="J3" s="12" t="s">
+      <c r="J3" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="K3" s="12" t="s">
+      <c r="K3" s="10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="2:11" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B4" s="15">
+    <row r="4" spans="2:11" ht="159" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="11">
         <v>1</v>
       </c>
-      <c r="C4" s="8"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="9"/>
-      <c r="K4" s="10"/>
-    </row>
-    <row r="5" spans="2:11" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B5" s="16">
+      <c r="C4" s="14">
+        <v>42864</v>
+      </c>
+      <c r="D4" s="15">
+        <v>42864</v>
+      </c>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="J4" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="K4" s="19" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="B5" s="12">
         <v>2</v>
       </c>
       <c r="C5" s="3"/>
@@ -799,8 +884,8 @@
       <c r="J5" s="2"/>
       <c r="K5" s="4"/>
     </row>
-    <row r="6" spans="2:11" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="16">
+    <row r="6" spans="2:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="B6" s="12">
         <v>3</v>
       </c>
       <c r="C6" s="3"/>
@@ -813,8 +898,8 @@
       <c r="J6" s="2"/>
       <c r="K6" s="4"/>
     </row>
-    <row r="7" spans="2:11" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B7" s="16">
+    <row r="7" spans="2:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="B7" s="12">
         <v>4</v>
       </c>
       <c r="C7" s="3"/>
@@ -827,8 +912,8 @@
       <c r="J7" s="2"/>
       <c r="K7" s="4"/>
     </row>
-    <row r="8" spans="2:11" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="16">
+    <row r="8" spans="2:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="B8" s="12">
         <v>5</v>
       </c>
       <c r="C8" s="3"/>
@@ -841,8 +926,8 @@
       <c r="J8" s="2"/>
       <c r="K8" s="4"/>
     </row>
-    <row r="9" spans="2:11" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="16">
+    <row r="9" spans="2:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="B9" s="12">
         <v>6</v>
       </c>
       <c r="C9" s="3"/>
@@ -855,8 +940,8 @@
       <c r="J9" s="2"/>
       <c r="K9" s="4"/>
     </row>
-    <row r="10" spans="2:11" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B10" s="16">
+    <row r="10" spans="2:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="B10" s="12">
         <v>7</v>
       </c>
       <c r="C10" s="3"/>
@@ -869,8 +954,8 @@
       <c r="J10" s="2"/>
       <c r="K10" s="4"/>
     </row>
-    <row r="11" spans="2:11" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B11" s="16">
+    <row r="11" spans="2:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="B11" s="12">
         <v>8</v>
       </c>
       <c r="C11" s="3"/>
@@ -883,8 +968,8 @@
       <c r="J11" s="2"/>
       <c r="K11" s="4"/>
     </row>
-    <row r="12" spans="2:11" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B12" s="16">
+    <row r="12" spans="2:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="B12" s="12">
         <v>9</v>
       </c>
       <c r="C12" s="3"/>
@@ -897,8 +982,8 @@
       <c r="J12" s="2"/>
       <c r="K12" s="4"/>
     </row>
-    <row r="13" spans="2:11" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B13" s="16">
+    <row r="13" spans="2:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="B13" s="12">
         <v>10</v>
       </c>
       <c r="C13" s="3"/>
@@ -911,8 +996,8 @@
       <c r="J13" s="2"/>
       <c r="K13" s="4"/>
     </row>
-    <row r="14" spans="2:11" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B14" s="16">
+    <row r="14" spans="2:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="B14" s="12">
         <v>11</v>
       </c>
       <c r="C14" s="3"/>
@@ -925,8 +1010,8 @@
       <c r="J14" s="2"/>
       <c r="K14" s="4"/>
     </row>
-    <row r="15" spans="2:11" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B15" s="16">
+    <row r="15" spans="2:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="B15" s="12">
         <v>12</v>
       </c>
       <c r="C15" s="3"/>
@@ -939,8 +1024,8 @@
       <c r="J15" s="2"/>
       <c r="K15" s="4"/>
     </row>
-    <row r="16" spans="2:11" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B16" s="16">
+    <row r="16" spans="2:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="B16" s="12">
         <v>13</v>
       </c>
       <c r="C16" s="3"/>
@@ -953,8 +1038,8 @@
       <c r="J16" s="2"/>
       <c r="K16" s="4"/>
     </row>
-    <row r="17" spans="2:11" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B17" s="16">
+    <row r="17" spans="2:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="B17" s="12">
         <v>14</v>
       </c>
       <c r="C17" s="3"/>
@@ -967,8 +1052,8 @@
       <c r="J17" s="2"/>
       <c r="K17" s="4"/>
     </row>
-    <row r="18" spans="2:11" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B18" s="16">
+    <row r="18" spans="2:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="B18" s="12">
         <v>15</v>
       </c>
       <c r="C18" s="3"/>
@@ -981,8 +1066,8 @@
       <c r="J18" s="2"/>
       <c r="K18" s="4"/>
     </row>
-    <row r="19" spans="2:11" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B19" s="16">
+    <row r="19" spans="2:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="B19" s="12">
         <v>16</v>
       </c>
       <c r="C19" s="3"/>
@@ -995,8 +1080,8 @@
       <c r="J19" s="2"/>
       <c r="K19" s="4"/>
     </row>
-    <row r="20" spans="2:11" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B20" s="16">
+    <row r="20" spans="2:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="B20" s="12">
         <v>17</v>
       </c>
       <c r="C20" s="3"/>
@@ -1009,8 +1094,8 @@
       <c r="J20" s="2"/>
       <c r="K20" s="4"/>
     </row>
-    <row r="21" spans="2:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="17">
+    <row r="21" spans="2:11" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B21" s="13">
         <v>18</v>
       </c>
       <c r="C21" s="5"/>
@@ -1023,8 +1108,8 @@
       <c r="J21" s="6"/>
       <c r="K21" s="7"/>
     </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B22" s="11"/>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B22" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1042,7 +1127,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1054,7 +1139,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>